<commit_message>
Worked out argparse and more playing around.
</commit_message>
<xml_diff>
--- a/Excel_read_serialnumber/Excel/Workbook.xlsx
+++ b/Excel_read_serialnumber/Excel/Workbook.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\python\Python-Projects\Excel_read_serialnumber\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74D3C09-09D8-4554-A101-78C2FEFFF422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5166E5A8-F4C1-4829-9E6F-4CA446C3BF90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27420" yWindow="960" windowWidth="23265" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="sheetnames" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -357,7 +356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -857,16 +856,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7504E289-91DB-42FE-91BC-7DB21AF93424}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Linkserial is now working!
</commit_message>
<xml_diff>
--- a/Excel_read_serialnumber/Excel/Workbook.xlsx
+++ b/Excel_read_serialnumber/Excel/Workbook.xlsx
@@ -1,54 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\python\Python-Projects\Excel_read_serialnumber\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5166E5A8-F4C1-4829-9E6F-4CA446C3BF90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27420" yWindow="960" windowWidth="23265" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-27420" yWindow="960" windowWidth="23265" windowHeight="12810" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Klant Serienummer</t>
-  </si>
-  <si>
-    <t>Matas QR</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -67,27 +46,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -353,507 +323,532 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col width="18.42578125" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="15.140625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Klant Serienummer</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Matas QR</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>60256</v>
       </c>
-      <c r="B2" s="2">
-        <v>19011200010001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>19011200020001</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>60257</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>19011200020002</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>60258</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>19011200020003</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>60259</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>19011200020004</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>60260</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>60261</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>60262</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>60263</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>60264</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="11">
+      <c r="A11" s="1" t="n">
         <v>60265</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12">
+      <c r="A12" s="1" t="n">
         <v>60266</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="13">
+      <c r="A13" s="1" t="n">
         <v>60267</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="14">
+      <c r="A14" s="1" t="n">
         <v>60268</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="15">
+      <c r="A15" s="1" t="n">
         <v>60269</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+    <row r="16">
+      <c r="A16" s="1" t="n">
         <v>60270</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="17">
+      <c r="A17" s="1" t="n">
         <v>60271</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+    <row r="18">
+      <c r="A18" s="1" t="n">
         <v>60272</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+    <row r="19">
+      <c r="A19" s="1" t="n">
         <v>60273</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+    <row r="20">
+      <c r="A20" s="1" t="n">
         <v>60274</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="21">
+      <c r="A21" s="1" t="n">
         <v>60275</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+    <row r="22">
+      <c r="A22" s="1" t="n">
         <v>60276</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23">
+      <c r="A23" s="1" t="n">
         <v>60277</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+    <row r="24">
+      <c r="A24" s="1" t="n">
         <v>60278</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+    <row r="25">
+      <c r="A25" s="1" t="n">
         <v>60279</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+    <row r="26">
+      <c r="A26" s="1" t="n">
         <v>60280</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+    <row r="27">
+      <c r="A27" s="1" t="n">
         <v>60281</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+    <row r="28">
+      <c r="A28" s="1" t="n">
         <v>60282</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+    <row r="29">
+      <c r="A29" s="1" t="n">
         <v>60283</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+    <row r="30">
+      <c r="A30" s="1" t="n">
         <v>60284</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+    <row r="31">
+      <c r="A31" s="1" t="n">
         <v>60285</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+    <row r="32">
+      <c r="A32" s="1" t="n">
         <v>60286</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+    <row r="33">
+      <c r="A33" s="1" t="n">
         <v>60287</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+    <row r="34">
+      <c r="A34" s="1" t="n">
         <v>60288</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+    <row r="35">
+      <c r="A35" s="1" t="n">
         <v>60289</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="36">
+      <c r="A36" s="1" t="n">
         <v>60290</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+    <row r="37">
+      <c r="A37" s="1" t="n">
         <v>60291</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+    <row r="38">
+      <c r="A38" s="1" t="n">
         <v>60292</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+    <row r="39">
+      <c r="A39" s="1" t="n">
         <v>60293</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+    <row r="40">
+      <c r="A40" s="1" t="n">
         <v>60294</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+    <row r="41">
+      <c r="A41" s="1" t="n">
         <v>60295</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="42">
+      <c r="A42" s="1" t="n">
         <v>60296</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+    <row r="43">
+      <c r="A43" s="1" t="n">
         <v>60297</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+    <row r="44">
+      <c r="A44" s="1" t="n">
         <v>60298</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+    <row r="45">
+      <c r="A45" s="1" t="n">
         <v>60299</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+    <row r="46">
+      <c r="A46" s="1" t="n">
         <v>60300</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+    <row r="47">
+      <c r="A47" s="1" t="n">
         <v>60301</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+    <row r="48">
+      <c r="A48" s="1" t="n">
         <v>60302</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+    <row r="49">
+      <c r="A49" s="1" t="n">
         <v>60303</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+    <row r="50">
+      <c r="A50" s="1" t="n">
         <v>60304</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+    <row r="51">
+      <c r="A51" s="1" t="n">
         <v>60305</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+    <row r="52">
+      <c r="A52" s="1" t="n">
         <v>60306</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+    <row r="53">
+      <c r="A53" s="1" t="n">
         <v>60307</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+    <row r="54">
+      <c r="A54" s="1" t="n">
         <v>60308</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+    <row r="55">
+      <c r="A55" s="1" t="n">
         <v>60309</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+    <row r="56">
+      <c r="A56" s="1" t="n">
         <v>60310</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+    <row r="57">
+      <c r="A57" s="1" t="n">
         <v>60311</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+    <row r="58">
+      <c r="A58" s="1" t="n">
         <v>60312</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+    <row r="59">
+      <c r="A59" s="1" t="n">
         <v>60313</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+    <row r="60">
+      <c r="A60" s="1" t="n">
         <v>60314</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+    <row r="61">
+      <c r="A61" s="1" t="n">
         <v>60315</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+    <row r="62">
+      <c r="A62" s="1" t="n">
         <v>60316</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+    <row r="63">
+      <c r="A63" s="1" t="n">
         <v>60317</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+    <row r="64">
+      <c r="A64" s="1" t="n">
         <v>60318</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+    <row r="65">
+      <c r="A65" s="1" t="n">
         <v>60319</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+    <row r="66">
+      <c r="A66" s="1" t="n">
         <v>60320</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+    <row r="67">
+      <c r="A67" s="1" t="n">
         <v>60321</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+    <row r="68">
+      <c r="A68" s="1" t="n">
         <v>60322</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+    <row r="69">
+      <c r="A69" s="1" t="n">
         <v>60323</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+    <row r="70">
+      <c r="A70" s="1" t="n">
         <v>60324</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+    <row r="71">
+      <c r="A71" s="1" t="n">
         <v>60325</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+    <row r="72">
+      <c r="A72" s="1" t="n">
         <v>60326</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+    <row r="73">
+      <c r="A73" s="1" t="n">
         <v>60327</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+    <row r="74">
+      <c r="A74" s="1" t="n">
         <v>60328</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+    <row r="75">
+      <c r="A75" s="1" t="n">
         <v>60329</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+    <row r="76">
+      <c r="A76" s="1" t="n">
         <v>60330</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+    <row r="77">
+      <c r="A77" s="1" t="n">
         <v>60331</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+    <row r="78">
+      <c r="A78" s="1" t="n">
         <v>60332</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+    <row r="79">
+      <c r="A79" s="1" t="n">
         <v>60333</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+    <row r="80">
+      <c r="A80" s="1" t="n">
         <v>60334</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+    <row r="81">
+      <c r="A81" s="1" t="n">
         <v>60335</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+    <row r="82">
+      <c r="A82" s="1" t="n">
         <v>60336</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+    <row r="83">
+      <c r="A83" s="1" t="n">
         <v>60337</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+    <row r="84">
+      <c r="A84" s="1" t="n">
         <v>60338</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+    <row r="85">
+      <c r="A85" s="1" t="n">
         <v>60339</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+    <row r="86">
+      <c r="A86" s="1" t="n">
         <v>60340</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+    <row r="87">
+      <c r="A87" s="1" t="n">
         <v>60341</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+    <row r="88">
+      <c r="A88" s="1" t="n">
         <v>60342</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+    <row r="89">
+      <c r="A89" s="1" t="n">
         <v>60343</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+    <row r="90">
+      <c r="A90" s="1" t="n">
         <v>60344</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+    <row r="91">
+      <c r="A91" s="1" t="n">
         <v>60345</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+    <row r="92">
+      <c r="A92" s="1" t="n">
         <v>60346</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+    <row r="93">
+      <c r="A93" s="1" t="n">
         <v>60347</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+    <row r="94">
+      <c r="A94" s="1" t="n">
         <v>60348</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+    <row r="95">
+      <c r="A95" s="1" t="n">
         <v>60349</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+    <row r="96">
+      <c r="A96" s="1" t="n">
         <v>60350</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Project done? Further testing required.
</commit_message>
<xml_diff>
--- a/Excel_read_serialnumber/Excel/Workbook.xlsx
+++ b/Excel_read_serialnumber/Excel/Workbook.xlsx
@@ -331,7 +331,7 @@
   <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -408,7 +408,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>19011200020006</t>
+          <t>19011200077777</t>
         </is>
       </c>
     </row>
@@ -418,7 +418,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>19011200020007</t>
+          <t>19011200077777</t>
         </is>
       </c>
     </row>
@@ -466,45 +466,90 @@
       <c r="A13" s="1" t="n">
         <v>60267</v>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19011200030003</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>60268</v>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>190112000777347</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>60269</v>
       </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>190112000777347</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>60270</v>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>190112000777347</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>60271</v>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>19011200076347</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>60272</v>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>19011200076347</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>60273</v>
       </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>19011200076347</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>60274</v>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>19011200076347</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>60275</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>19011200076347</t>
+        </is>
       </c>
     </row>
     <row r="22">

</xml_diff>